<commit_message>
add column header for outcome
</commit_message>
<xml_diff>
--- a/Assoc. of WA Cities Signatories/Federal Way - 2nd PDR sent/Data/Color-coded copy of 2019-2023 Vehicle Pursuit Search (1).xlsx
+++ b/Assoc. of WA Cities Signatories/Federal Way - 2nd PDR sent/Data/Color-coded copy of 2019-2023 Vehicle Pursuit Search (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whobbs\Desktop\JUSTFOIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\wa-pursuit-pdr-data\Assoc. of WA Cities Signatories\Federal Way - 2nd PDR sent\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10BEF291-E1B7-4EA5-82B8-C552EBC1CAE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DFFFBA-A874-48DE-AAC9-2C140BBBFA7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22155" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Records" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="197">
   <si>
     <t>Incident</t>
   </si>
@@ -621,6 +621,9 @@
   </si>
   <si>
     <t>*Pursuit; FWPD joined an outside agency pursuit that had a single officer in the pursuit, lost vehicle.*</t>
+  </si>
+  <si>
+    <t>Outcome</t>
   </si>
 </sst>
 </file>
@@ -766,6 +769,7 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1117,7 +1121,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1479,7 +1483,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,6 +1524,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>